<commit_message>
rename major query column to type
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\trialsurveillanceapp\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D752720-C5A9-40E4-B1A0-85F96D056DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB826BA-A596-4334-BE07-E00425A84804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="6" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_specs" sheetId="17" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="317">
   <si>
     <t>continuous</t>
   </si>
@@ -1018,6 +1018,12 @@
   </si>
   <si>
     <t>name_new</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -1191,8 +1197,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}" name="Table26" displayName="Table26" ref="A1:B14" totalsRowShown="0">
-  <autoFilter ref="A1:B14" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}" name="Table26" displayName="Table26" ref="A1:B15" totalsRowShown="0">
+  <autoFilter ref="A1:B15" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B14">
     <sortCondition ref="B1:B14"/>
   </sortState>
@@ -1503,18 +1509,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A2BBF1-D698-4542-9229-382D48A2C041}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>313</v>
       </c>
@@ -1525,7 +1531,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>293</v>
       </c>
@@ -1536,7 +1542,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -1547,7 +1553,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>295</v>
       </c>
@@ -1558,7 +1564,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>296</v>
       </c>
@@ -1569,7 +1575,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>297</v>
       </c>
@@ -1580,7 +1586,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>298</v>
       </c>
@@ -1591,7 +1597,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>299</v>
       </c>
@@ -1602,7 +1608,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>300</v>
       </c>
@@ -1613,7 +1619,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>301</v>
       </c>
@@ -1624,7 +1630,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>302</v>
       </c>
@@ -1635,7 +1641,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>303</v>
       </c>
@@ -1662,14 +1668,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1680,7 +1686,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1691,7 +1697,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1702,7 +1708,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1713,7 +1719,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1724,7 +1730,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1735,7 +1741,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1746,7 +1752,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1757,7 +1763,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1768,7 +1774,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1779,7 +1785,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1790,7 +1796,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1801,7 +1807,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1812,7 +1818,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1823,7 +1829,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1834,7 +1840,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1845,7 +1851,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1856,7 +1862,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1867,7 +1873,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1878,7 +1884,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1906,20 +1912,20 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1936,7 +1942,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -1950,7 +1956,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1964,7 +1970,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1978,7 +1984,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -1992,7 +1998,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -2006,7 +2012,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -2020,7 +2026,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -2034,7 +2040,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -2048,7 +2054,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -2062,7 +2068,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -2076,7 +2082,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -2090,7 +2096,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -2104,7 +2110,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>258</v>
       </c>
@@ -2118,7 +2124,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -2132,7 +2138,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -2146,7 +2152,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>250</v>
       </c>
@@ -2160,7 +2166,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -2174,7 +2180,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>123</v>
       </c>
@@ -2188,7 +2194,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -2202,7 +2208,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>160</v>
       </c>
@@ -2216,7 +2222,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -2230,7 +2236,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>217</v>
       </c>
@@ -2244,7 +2250,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>251</v>
       </c>
@@ -2258,7 +2264,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>166</v>
       </c>
@@ -2272,7 +2278,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>168</v>
       </c>
@@ -2286,7 +2292,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>170</v>
       </c>
@@ -2300,7 +2306,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>172</v>
       </c>
@@ -2314,7 +2320,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>174</v>
       </c>
@@ -2328,7 +2334,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>176</v>
       </c>
@@ -2342,7 +2348,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>177</v>
       </c>
@@ -2356,7 +2362,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>180</v>
       </c>
@@ -2370,7 +2376,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>182</v>
       </c>
@@ -2384,7 +2390,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>184</v>
       </c>
@@ -2398,7 +2404,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>164</v>
       </c>
@@ -2412,7 +2418,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>165</v>
       </c>
@@ -2426,7 +2432,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>186</v>
       </c>
@@ -2440,7 +2446,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>188</v>
       </c>
@@ -2454,7 +2460,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>189</v>
       </c>
@@ -2468,7 +2474,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>197</v>
       </c>
@@ -2482,7 +2488,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>199</v>
       </c>
@@ -2496,7 +2502,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>200</v>
       </c>
@@ -2510,7 +2516,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>191</v>
       </c>
@@ -2524,7 +2530,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>192</v>
       </c>
@@ -2538,7 +2544,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>203</v>
       </c>
@@ -2552,7 +2558,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>206</v>
       </c>
@@ -2566,7 +2572,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>207</v>
       </c>
@@ -2580,7 +2586,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>209</v>
       </c>
@@ -2594,7 +2600,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>211</v>
       </c>
@@ -2608,7 +2614,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>213</v>
       </c>
@@ -2622,7 +2628,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>214</v>
       </c>
@@ -2653,23 +2659,23 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2695,7 +2701,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -2712,7 +2718,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -2729,7 +2735,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -2746,7 +2752,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -2763,7 +2769,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -2780,7 +2786,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -2797,7 +2803,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -2814,7 +2820,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -2831,7 +2837,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -2848,7 +2854,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -2865,7 +2871,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2882,7 +2888,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -2899,7 +2905,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2916,7 +2922,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -2942,7 +2948,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -2968,7 +2974,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -2994,7 +3000,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -3020,7 +3026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -3046,7 +3052,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -3063,7 +3069,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -3089,7 +3095,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -3115,7 +3121,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -3132,7 +3138,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -3149,7 +3155,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -3166,7 +3172,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -3183,7 +3189,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -3200,7 +3206,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -3217,7 +3223,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>246</v>
       </c>
@@ -3231,7 +3237,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>247</v>
       </c>
@@ -3262,20 +3268,20 @@
       <selection activeCell="E8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3292,7 +3298,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -3306,7 +3312,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -3320,7 +3326,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -3334,7 +3340,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -3348,7 +3354,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -3362,7 +3368,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -3376,7 +3382,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -3390,7 +3396,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -3404,7 +3410,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -3418,7 +3424,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>133</v>
       </c>
@@ -3432,7 +3438,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -3446,7 +3452,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -3460,7 +3466,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -3474,7 +3480,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -3488,7 +3494,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>141</v>
       </c>
@@ -3502,7 +3508,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -3516,7 +3522,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -3530,7 +3536,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>138</v>
       </c>
@@ -3544,7 +3550,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -3558,7 +3564,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -3589,15 +3595,15 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>244</v>
       </c>
@@ -3611,7 +3617,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -3625,7 +3631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -3639,7 +3645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -3653,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -3667,7 +3673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -3681,7 +3687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -3706,19 +3712,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FFF7FA-E437-4B11-81D1-BE338C7C5391}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>269</v>
       </c>
@@ -3726,7 +3732,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>282</v>
       </c>
@@ -3734,7 +3740,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>289</v>
       </c>
@@ -3742,7 +3748,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>280</v>
       </c>
@@ -3750,7 +3756,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>280</v>
       </c>
@@ -3758,7 +3764,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>287</v>
       </c>
@@ -3766,7 +3772,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>272</v>
       </c>
@@ -3774,7 +3780,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>277</v>
       </c>
@@ -3782,7 +3788,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>279</v>
       </c>
@@ -3790,7 +3796,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>291</v>
       </c>
@@ -3798,7 +3804,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>284</v>
       </c>
@@ -3806,7 +3812,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>271</v>
       </c>
@@ -3814,7 +3820,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>274</v>
       </c>
@@ -3822,12 +3828,20 @@
         <v>273</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>285</v>
       </c>
       <c r="B14" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>315</v>
+      </c>
+      <c r="B15" t="s">
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renaming the metadata tab `column_specs` to the more fitting name `column_names` (since column specs are now internal)
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\trialsurveillanceapp\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB826BA-A596-4334-BE07-E00425A84804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B25D667-A405-49E2-BA00-076698E25281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="6" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
-    <sheet name="column_specs" sheetId="17" r:id="rId1"/>
+    <sheet name="column_names" sheetId="17" r:id="rId1"/>
     <sheet name="events" sheetId="1" r:id="rId2"/>
     <sheet name="common_forms" sheetId="13" r:id="rId3"/>
     <sheet name="study_forms" sheetId="14" r:id="rId4"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="312">
   <si>
     <t>continuous</t>
   </si>
@@ -951,9 +951,6 @@
     <t>Author</t>
   </si>
   <si>
-    <t>col_type</t>
-  </si>
-  <si>
     <t>SiteCode</t>
   </si>
   <si>
@@ -1000,18 +997,6 @@
   </si>
   <si>
     <t>form_repeat</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>T</t>
   </si>
   <si>
     <t>name_raw</t>
@@ -1110,12 +1095,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}" name="Table7" displayName="Table7" ref="A1:C12" totalsRowShown="0">
-  <autoFilter ref="A1:C12" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}" name="Table7" displayName="Table7" ref="A1:B12" totalsRowShown="0">
+  <autoFilter ref="A1:B12" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{197420D8-A12C-4324-87A4-2BEAC3F2FAF6}" name="name_raw"/>
     <tableColumn id="2" xr3:uid="{9CEB246F-9418-43C1-93E4-E01091B6A441}" name="name_new"/>
-    <tableColumn id="3" xr3:uid="{02ABA40F-2623-4142-A00F-3D3C95D63E14}" name="col_type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1507,149 +1491,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A2BBF1-D698-4542-9229-382D48A2C041}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>293</v>
-      </c>
-      <c r="B2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>294</v>
       </c>
       <c r="B3" t="s">
         <v>270</v>
       </c>
-      <c r="C3" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>295</v>
-      </c>
-      <c r="B4" t="s">
-        <v>305</v>
-      </c>
-      <c r="C4" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>296</v>
       </c>
       <c r="B5" t="s">
         <v>288</v>
       </c>
-      <c r="C5" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B6" t="s">
         <v>268</v>
       </c>
-      <c r="C6" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B7" t="s">
         <v>286</v>
       </c>
-      <c r="C7" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>299</v>
       </c>
-      <c r="B8" t="s">
-        <v>306</v>
-      </c>
-      <c r="C8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>300</v>
-      </c>
-      <c r="B9" t="s">
-        <v>308</v>
-      </c>
-      <c r="C9" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>301</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>301</v>
+      </c>
+      <c r="B11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>302</v>
-      </c>
-      <c r="B11" t="s">
-        <v>307</v>
-      </c>
-      <c r="C11" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>303</v>
       </c>
       <c r="B12" t="s">
         <v>281</v>
-      </c>
-      <c r="C12" t="s">
-        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -1668,14 +1613,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1686,7 +1631,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1697,7 +1642,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1708,7 +1653,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1719,7 +1664,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1730,7 +1675,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1741,7 +1686,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1752,7 +1697,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1763,7 +1708,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1774,7 +1719,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1785,7 +1730,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1796,7 +1741,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1807,7 +1752,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1818,7 +1763,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1829,7 +1774,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1840,7 +1785,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1851,7 +1796,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1862,7 +1807,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1873,7 +1818,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1884,7 +1829,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1912,20 +1857,20 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1942,7 +1887,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -1956,7 +1901,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1970,7 +1915,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1984,7 +1929,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -1998,7 +1943,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -2012,7 +1957,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -2026,7 +1971,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -2040,7 +1985,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -2054,7 +1999,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -2068,7 +2013,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -2082,7 +2027,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -2096,7 +2041,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -2110,7 +2055,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>258</v>
       </c>
@@ -2124,7 +2069,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -2138,7 +2083,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -2152,7 +2097,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>250</v>
       </c>
@@ -2166,7 +2111,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -2180,7 +2125,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>123</v>
       </c>
@@ -2194,7 +2139,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -2208,7 +2153,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>160</v>
       </c>
@@ -2222,7 +2167,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -2236,7 +2181,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>217</v>
       </c>
@@ -2250,7 +2195,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>251</v>
       </c>
@@ -2264,7 +2209,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>166</v>
       </c>
@@ -2278,7 +2223,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>168</v>
       </c>
@@ -2292,7 +2237,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>170</v>
       </c>
@@ -2306,7 +2251,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>172</v>
       </c>
@@ -2320,7 +2265,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>174</v>
       </c>
@@ -2334,7 +2279,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>176</v>
       </c>
@@ -2348,7 +2293,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>177</v>
       </c>
@@ -2362,7 +2307,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>180</v>
       </c>
@@ -2376,7 +2321,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>182</v>
       </c>
@@ -2390,7 +2335,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>184</v>
       </c>
@@ -2404,7 +2349,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>164</v>
       </c>
@@ -2418,7 +2363,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>165</v>
       </c>
@@ -2432,7 +2377,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>186</v>
       </c>
@@ -2446,7 +2391,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>188</v>
       </c>
@@ -2460,7 +2405,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>189</v>
       </c>
@@ -2474,7 +2419,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>197</v>
       </c>
@@ -2488,7 +2433,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>199</v>
       </c>
@@ -2502,7 +2447,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>200</v>
       </c>
@@ -2516,7 +2461,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>191</v>
       </c>
@@ -2530,7 +2475,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>192</v>
       </c>
@@ -2544,7 +2489,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>203</v>
       </c>
@@ -2558,7 +2503,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>206</v>
       </c>
@@ -2572,7 +2517,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>207</v>
       </c>
@@ -2586,7 +2531,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>209</v>
       </c>
@@ -2600,7 +2545,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>211</v>
       </c>
@@ -2614,7 +2559,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>213</v>
       </c>
@@ -2628,7 +2573,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>214</v>
       </c>
@@ -2659,23 +2604,23 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="26.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2701,7 +2646,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -2718,7 +2663,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -2735,7 +2680,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -2752,7 +2697,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -2769,7 +2714,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -2786,7 +2731,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -2803,7 +2748,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -2820,7 +2765,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -2837,7 +2782,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -2854,7 +2799,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -2871,7 +2816,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2888,7 +2833,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -2905,7 +2850,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>54</v>
       </c>
@@ -2922,7 +2867,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -2948,7 +2893,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -2974,7 +2919,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -3000,7 +2945,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -3026,7 +2971,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -3052,7 +2997,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -3069,7 +3014,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -3095,7 +3040,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -3121,7 +3066,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -3138,7 +3083,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -3155,7 +3100,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -3172,7 +3117,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -3189,7 +3134,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -3206,7 +3151,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -3223,7 +3168,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>246</v>
       </c>
@@ -3237,7 +3182,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>247</v>
       </c>
@@ -3268,20 +3213,20 @@
       <selection activeCell="E8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3298,7 +3243,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -3312,7 +3257,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -3326,7 +3271,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -3340,7 +3285,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -3354,7 +3299,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -3368,7 +3313,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -3382,7 +3327,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -3396,7 +3341,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -3410,7 +3355,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -3424,7 +3369,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>133</v>
       </c>
@@ -3438,7 +3383,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -3452,7 +3397,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -3466,7 +3411,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -3480,7 +3425,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -3494,7 +3439,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>141</v>
       </c>
@@ -3508,7 +3453,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -3522,7 +3467,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -3536,7 +3481,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>138</v>
       </c>
@@ -3550,7 +3495,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -3564,7 +3509,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -3595,15 +3540,15 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>244</v>
       </c>
@@ -3617,7 +3562,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -3631,7 +3576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -3645,7 +3590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -3659,7 +3604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -3673,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -3687,7 +3632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -3714,17 +3659,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FFF7FA-E437-4B11-81D1-BE338C7C5391}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>269</v>
       </c>
@@ -3732,7 +3677,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>282</v>
       </c>
@@ -3740,7 +3685,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>289</v>
       </c>
@@ -3748,7 +3693,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>280</v>
       </c>
@@ -3756,7 +3701,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>280</v>
       </c>
@@ -3764,7 +3709,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>287</v>
       </c>
@@ -3772,7 +3717,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>272</v>
       </c>
@@ -3780,7 +3725,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>277</v>
       </c>
@@ -3788,7 +3733,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>279</v>
       </c>
@@ -3796,7 +3741,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>291</v>
       </c>
@@ -3804,7 +3749,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>284</v>
       </c>
@@ -3812,7 +3757,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>271</v>
       </c>
@@ -3820,7 +3765,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>274</v>
       </c>
@@ -3828,7 +3773,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>285</v>
       </c>
@@ -3836,12 +3781,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B15" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update metadata.xlsx, renaming the groups tab to form_level_data, add 'review_required' column, and create new metadata with updated get_metadata() function
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B25D667-A405-49E2-BA00-076698E25281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDAC79F-56F2-4323-B98E-863161773ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="common_forms" sheetId="13" r:id="rId3"/>
     <sheet name="study_forms" sheetId="14" r:id="rId4"/>
     <sheet name="general" sheetId="15" r:id="rId5"/>
-    <sheet name="groups" sheetId="11" r:id="rId6"/>
+    <sheet name="form_level_data" sheetId="11" r:id="rId6"/>
     <sheet name="table_names" sheetId="16" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="313">
   <si>
     <t>continuous</t>
   </si>
@@ -1009,6 +1009,9 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>review_required</t>
   </si>
 </sst>
 </file>
@@ -1172,9 +1175,9 @@
   <autoFilter ref="A1:D7" xr:uid="{7AED27C5-CB47-4830-8F47-BB9354073F14}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D16F68B8-5C50-48F1-9AAD-869306EF0109}" name="item_group"/>
-    <tableColumn id="6" xr3:uid="{25505D7A-1975-43B2-936F-BEF9951B7B1C}" name="item_type"/>
     <tableColumn id="3" xr3:uid="{C44DD745-DA94-43D6-993D-55FB6C28A7E6}" name="item_scale"/>
     <tableColumn id="5" xr3:uid="{8D42B0BE-426B-4694-A11B-9C5E9C7F7CA2}" name="use_unscaled_limits"/>
+    <tableColumn id="2" xr3:uid="{B00F83D4-EB53-40B2-8D95-A5BD73B72F5F}" name="review_required"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1493,7 +1496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A2BBF1-D698-4542-9229-382D48A2C041}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1853,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2EDD7A-5ED3-4521-BBD0-E5535A4AFBF0}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2600,8 +2603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB3F453-AEAC-4610-ADFE-EC9F8781793B}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2646,427 +2649,427 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2">
+        <v>90</v>
+      </c>
+      <c r="H2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3">
+        <v>55</v>
+      </c>
+      <c r="H3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6">
+        <v>35</v>
+      </c>
+      <c r="H6">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8">
+        <v>18.5</v>
+      </c>
+      <c r="H8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>45</v>
+      </c>
+      <c r="H9">
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15">
-        <v>90</v>
-      </c>
-      <c r="H15">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16">
-        <v>55</v>
-      </c>
-      <c r="H16">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17">
-        <v>60</v>
-      </c>
-      <c r="H17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18">
-        <v>12</v>
-      </c>
-      <c r="H18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19">
-        <v>35</v>
-      </c>
-      <c r="H19">
-        <v>38.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21">
-        <v>18.5</v>
-      </c>
-      <c r="H21">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22">
-        <v>45</v>
-      </c>
-      <c r="H22">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -3083,7 +3086,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -3100,7 +3103,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -3117,7 +3120,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -3134,7 +3137,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -3151,7 +3154,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -3168,7 +3171,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>246</v>
       </c>
@@ -3182,7 +3185,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>247</v>
       </c>
@@ -3537,15 +3540,16 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -3553,24 +3557,24 @@
         <v>244</v>
       </c>
       <c r="B1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C1" t="s">
-        <v>245</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>98</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="b">
         <v>0</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -3580,39 +3584,39 @@
       <c r="A3" t="s">
         <v>68</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="b">
         <v>0</v>
       </c>
-      <c r="C3" t="b">
+      <c r="D3" t="b">
         <v>1</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="b">
         <v>0</v>
       </c>
-      <c r="C4" t="b">
+      <c r="D4" t="b">
         <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" t="b">
         <v>0</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -3622,28 +3626,28 @@
       <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
         <v>0</v>
       </c>
-      <c r="C6" t="b">
+      <c r="D6" t="b">
         <v>1</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>93</v>
       </c>
-      <c r="B7" t="s">
-        <v>40</v>
+      <c r="B7" t="b">
+        <v>0</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change metadata table_names: form_repeat will now show as 'N' in a custom DT
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDAC79F-56F2-4323-B98E-863161773ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30574667-4508-48B2-A7D3-CCFA93E36DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="314">
   <si>
     <t>continuous</t>
   </si>
@@ -1012,6 +1012,9 @@
   </si>
   <si>
     <t>review_required</t>
+  </si>
+  <si>
+    <t>eN</t>
   </si>
 </sst>
 </file>
@@ -1184,10 +1187,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}" name="Table26" displayName="Table26" ref="A1:B15" totalsRowShown="0">
-  <autoFilter ref="A1:B15" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B14">
-    <sortCondition ref="B1:B14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}" name="Table26" displayName="Table26" ref="A1:B16" totalsRowShown="0">
+  <autoFilter ref="A1:B16" xr:uid="{9EDD03AE-80CB-44E4-BEA7-CD03D0476EFD}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
+    <sortCondition ref="B1:B15"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{728B9066-E1CE-4216-8337-A4FCDD0B5972}" name="table_name"/>
@@ -1496,7 +1499,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A2BBF1-D698-4542-9229-382D48A2C041}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2603,7 +2608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB3F453-AEAC-4610-ADFE-EC9F8781793B}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -3661,10 +3666,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FFF7FA-E437-4B11-81D1-BE338C7C5391}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3715,7 +3720,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>287</v>
+        <v>313</v>
       </c>
       <c r="B6" t="s">
         <v>286</v>
@@ -3731,65 +3736,73 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="B8" t="s">
-        <v>276</v>
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="B10" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="B11" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="B12" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B13" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>285</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>310</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>311</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Move additional merging functions to metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jthompson\Documents\R Projects\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30574667-4508-48B2-A7D3-CCFA93E36DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97B3513-CBE7-4971-809F-39F22B68361F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="-57720" yWindow="-2085" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="general" sheetId="15" r:id="rId5"/>
     <sheet name="form_level_data" sheetId="11" r:id="rId6"/>
     <sheet name="table_names" sheetId="16" r:id="rId7"/>
+    <sheet name="settings" sheetId="18" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="316">
   <si>
     <t>continuous</t>
   </si>
@@ -1015,6 +1016,12 @@
   </si>
   <si>
     <t>eN</t>
+  </si>
+  <si>
+    <t>add_fns</t>
+  </si>
+  <si>
+    <t>apply_study_specific_fixes</t>
   </si>
 </sst>
 </file>
@@ -1503,13 +1510,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>308</v>
       </c>
@@ -1517,7 +1524,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>292</v>
       </c>
@@ -1525,7 +1532,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>293</v>
       </c>
@@ -1533,7 +1540,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -1541,7 +1548,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>295</v>
       </c>
@@ -1549,7 +1556,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>296</v>
       </c>
@@ -1557,7 +1564,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>297</v>
       </c>
@@ -1565,7 +1572,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>298</v>
       </c>
@@ -1573,7 +1580,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>299</v>
       </c>
@@ -1581,7 +1588,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>300</v>
       </c>
@@ -1589,7 +1596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>301</v>
       </c>
@@ -1597,7 +1604,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>302</v>
       </c>
@@ -1621,14 +1628,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1639,7 +1646,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1650,7 +1657,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1661,7 +1668,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1672,7 +1679,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1683,7 +1690,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1694,7 +1701,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1705,7 +1712,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1716,7 +1723,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1727,7 +1734,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1738,7 +1745,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1749,7 +1756,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1760,7 +1767,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1771,7 +1778,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1782,7 +1789,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1793,7 +1800,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1804,7 +1811,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1815,7 +1822,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1826,7 +1833,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1837,7 +1844,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1865,20 +1872,20 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1895,7 +1902,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -1909,7 +1916,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1923,7 +1930,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1937,7 +1944,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -1951,7 +1958,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -1965,7 +1972,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -1979,7 +1986,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -1993,7 +2000,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -2007,7 +2014,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -2021,7 +2028,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -2035,7 +2042,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -2049,7 +2056,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -2063,7 +2070,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>258</v>
       </c>
@@ -2077,7 +2084,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -2091,7 +2098,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -2105,7 +2112,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>250</v>
       </c>
@@ -2119,7 +2126,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -2133,7 +2140,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>123</v>
       </c>
@@ -2147,7 +2154,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -2161,7 +2168,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>160</v>
       </c>
@@ -2175,7 +2182,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -2189,7 +2196,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>217</v>
       </c>
@@ -2203,7 +2210,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>251</v>
       </c>
@@ -2217,7 +2224,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>166</v>
       </c>
@@ -2231,7 +2238,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>168</v>
       </c>
@@ -2245,7 +2252,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>170</v>
       </c>
@@ -2259,7 +2266,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>172</v>
       </c>
@@ -2273,7 +2280,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>174</v>
       </c>
@@ -2287,7 +2294,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>176</v>
       </c>
@@ -2301,7 +2308,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>177</v>
       </c>
@@ -2315,7 +2322,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>180</v>
       </c>
@@ -2329,7 +2336,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>182</v>
       </c>
@@ -2343,7 +2350,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>184</v>
       </c>
@@ -2357,7 +2364,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>164</v>
       </c>
@@ -2371,7 +2378,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>165</v>
       </c>
@@ -2385,7 +2392,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>186</v>
       </c>
@@ -2399,7 +2406,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>188</v>
       </c>
@@ -2413,7 +2420,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>189</v>
       </c>
@@ -2427,7 +2434,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>197</v>
       </c>
@@ -2441,7 +2448,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>199</v>
       </c>
@@ -2455,7 +2462,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>200</v>
       </c>
@@ -2469,7 +2476,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>191</v>
       </c>
@@ -2483,7 +2490,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>192</v>
       </c>
@@ -2497,7 +2504,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>203</v>
       </c>
@@ -2511,7 +2518,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>206</v>
       </c>
@@ -2525,7 +2532,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>207</v>
       </c>
@@ -2539,7 +2546,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>209</v>
       </c>
@@ -2553,7 +2560,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>211</v>
       </c>
@@ -2567,7 +2574,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>213</v>
       </c>
@@ -2581,7 +2588,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>214</v>
       </c>
@@ -2612,23 +2619,23 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2654,7 +2661,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -2680,7 +2687,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -2706,7 +2713,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -2732,7 +2739,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2758,7 +2765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -2784,7 +2791,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -2801,7 +2808,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2827,7 +2834,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -2853,7 +2860,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -2870,7 +2877,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -2887,7 +2894,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2904,7 +2911,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -2921,7 +2928,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -2938,7 +2945,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2955,7 +2962,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -2972,7 +2979,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -2989,7 +2996,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -3006,7 +3013,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -3023,7 +3030,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -3040,7 +3047,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -3057,7 +3064,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -3074,7 +3081,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -3091,7 +3098,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -3108,7 +3115,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -3125,7 +3132,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -3142,7 +3149,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -3159,7 +3166,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -3176,7 +3183,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>246</v>
       </c>
@@ -3190,7 +3197,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>247</v>
       </c>
@@ -3221,20 +3228,20 @@
       <selection activeCell="E8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3251,7 +3258,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -3265,7 +3272,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -3279,7 +3286,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -3293,7 +3300,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -3307,7 +3314,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -3321,7 +3328,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -3335,7 +3342,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -3349,7 +3356,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -3363,7 +3370,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -3377,7 +3384,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>133</v>
       </c>
@@ -3391,7 +3398,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -3405,7 +3412,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -3419,7 +3426,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -3433,7 +3440,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -3447,7 +3454,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>141</v>
       </c>
@@ -3461,7 +3468,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -3475,7 +3482,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -3489,7 +3496,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>138</v>
       </c>
@@ -3503,7 +3510,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -3517,7 +3524,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -3548,16 +3555,16 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>244</v>
       </c>
@@ -3571,7 +3578,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -3585,7 +3592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -3599,7 +3606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -3613,7 +3620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -3627,7 +3634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -3641,7 +3648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -3668,17 +3675,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9FFF7FA-E437-4B11-81D1-BE338C7C5391}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>269</v>
       </c>
@@ -3686,7 +3693,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>282</v>
       </c>
@@ -3694,7 +3701,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>289</v>
       </c>
@@ -3702,7 +3709,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>280</v>
       </c>
@@ -3710,7 +3717,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>280</v>
       </c>
@@ -3718,7 +3725,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>313</v>
       </c>
@@ -3726,7 +3733,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>272</v>
       </c>
@@ -3734,7 +3741,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>287</v>
       </c>
@@ -3742,7 +3749,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>277</v>
       </c>
@@ -3750,7 +3757,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>279</v>
       </c>
@@ -3758,7 +3765,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>291</v>
       </c>
@@ -3766,7 +3773,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>284</v>
       </c>
@@ -3774,7 +3781,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>271</v>
       </c>
@@ -3782,7 +3789,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>274</v>
       </c>
@@ -3790,7 +3797,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>285</v>
       </c>
@@ -3798,7 +3805,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>310</v>
       </c>
@@ -3811,6 +3818,34 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2F7ED2-3887-47C4-B9C3-26B3456EF3BF}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Specify `add_fns` as `post_merge_fns`
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jthompson\Documents\R Projects\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97B3513-CBE7-4971-809F-39F22B68361F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71966C39-CDFF-4A14-83F6-338A95CDD680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-2085" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="-67320" yWindow="1560" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="317">
   <si>
     <t>continuous</t>
   </si>
@@ -1018,10 +1018,13 @@
     <t>eN</t>
   </si>
   <si>
-    <t>add_fns</t>
-  </si>
-  <si>
     <t>apply_study_specific_fixes</t>
+  </si>
+  <si>
+    <t>post_merge_fns</t>
+  </si>
+  <si>
+    <t>pre_merge_fns</t>
   </si>
 </sst>
 </file>
@@ -3823,25 +3826,29 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2F7ED2-3887-47C4-B9C3-26B3456EF3BF}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Impute `event_name` from `event` instead of `event_name`
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jthompson\Documents\R Projects\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71966C39-CDFF-4A14-83F6-338A95CDD680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08CFCF0-CB34-4E41-A382-689366DE8F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-67320" yWindow="1560" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="-67320" yWindow="1560" windowWidth="29040" windowHeight="15720" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="318">
   <si>
     <t>continuous</t>
   </si>
@@ -1025,6 +1025,9 @@
   </si>
   <si>
     <t>pre_merge_fns</t>
+  </si>
+  <si>
+    <t>event</t>
   </si>
 </sst>
 </file>
@@ -1509,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A2BBF1-D698-4542-9229-382D48A2C041}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1564,7 +1567,7 @@
         <v>296</v>
       </c>
       <c r="B6" t="s">
-        <v>268</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -3828,7 +3831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2F7ED2-3887-47C4-B9C3-26B3456EF3BF}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove `event_name` from required columns
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jthompson\Documents\R Projects\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C4F2CE-0D64-4EA2-9E03-E848EFA50D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4443961-4519-4AE4-BDD9-08EC50D20B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-67320" yWindow="1560" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="-67320" yWindow="1560" windowWidth="29040" windowHeight="15720" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="318">
   <si>
     <t>continuous</t>
   </si>
@@ -964,9 +964,6 @@
     <t>EventDate</t>
   </si>
   <si>
-    <t>EventName</t>
-  </si>
-  <si>
     <t>EventSeq</t>
   </si>
   <si>
@@ -1025,9 +1022,6 @@
   </si>
   <si>
     <t>pre_merge_fns</t>
-  </si>
-  <si>
-    <t>event</t>
   </si>
   <si>
     <t>mid_merge_fns</t>
@@ -1120,8 +1114,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}" name="Table7" displayName="Table7" ref="A1:B12" totalsRowShown="0">
-  <autoFilter ref="A1:B12" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}" name="Table7" displayName="Table7" ref="A1:B11" totalsRowShown="0">
+  <autoFilter ref="A1:B11" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{197420D8-A12C-4324-87A4-2BEAC3F2FAF6}" name="name_raw"/>
     <tableColumn id="2" xr3:uid="{9CEB246F-9418-43C1-93E4-E01091B6A441}" name="name_new"/>
@@ -1516,11 +1510,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A2BBF1-D698-4542-9229-382D48A2C041}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1530,10 +1522,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" t="s">
         <v>308</v>
-      </c>
-      <c r="B1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1541,7 +1533,7 @@
         <v>292</v>
       </c>
       <c r="B2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1557,7 +1549,7 @@
         <v>294</v>
       </c>
       <c r="B4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1573,7 +1565,7 @@
         <v>296</v>
       </c>
       <c r="B6" t="s">
-        <v>317</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1581,7 +1573,7 @@
         <v>297</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1589,7 +1581,7 @@
         <v>298</v>
       </c>
       <c r="B8" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1597,7 +1589,7 @@
         <v>299</v>
       </c>
       <c r="B9" t="s">
-        <v>307</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1605,7 +1597,7 @@
         <v>300</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1613,14 +1605,6 @@
         <v>301</v>
       </c>
       <c r="B11" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>302</v>
-      </c>
-      <c r="B12" t="s">
         <v>281</v>
       </c>
     </row>
@@ -3587,7 +3571,7 @@
         <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -3739,7 +3723,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B6" t="s">
         <v>286</v>
@@ -3758,7 +3742,7 @@
         <v>287</v>
       </c>
       <c r="B8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -3819,10 +3803,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>309</v>
+      </c>
+      <c r="B16" t="s">
         <v>310</v>
-      </c>
-      <c r="B16" t="s">
-        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -3837,7 +3821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2F7ED2-3887-47C4-B9C3-26B3456EF3BF}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3848,21 +3832,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B1" t="s">
         <v>316</v>
       </c>
-      <c r="B1" t="s">
-        <v>318</v>
-      </c>
       <c r="C1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make treatment label name a setting in the Excel metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jthompson\Documents\R Projects\clinsight\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CD744A-DA6C-4790-8B78-CF8C615FB65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A40C8F-9D5D-435B-8360-C25C0BBE8E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-67320" yWindow="1560" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="322">
   <si>
     <t>continuous</t>
   </si>
@@ -1034,6 +1034,12 @@
   </si>
   <si>
     <t>apply_edc_specific_changes</t>
+  </si>
+  <si>
+    <t>treatment_label</t>
+  </si>
+  <si>
+    <t>\U1F48A T\U2093</t>
   </si>
 </sst>
 </file>
@@ -1520,13 +1526,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>307</v>
       </c>
@@ -1534,7 +1540,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>292</v>
       </c>
@@ -1542,7 +1548,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>293</v>
       </c>
@@ -1550,7 +1556,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -1558,7 +1564,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>295</v>
       </c>
@@ -1566,7 +1572,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>296</v>
       </c>
@@ -1574,7 +1580,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>297</v>
       </c>
@@ -1582,7 +1588,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>298</v>
       </c>
@@ -1590,7 +1596,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>299</v>
       </c>
@@ -1598,7 +1604,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>300</v>
       </c>
@@ -1606,7 +1612,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>301</v>
       </c>
@@ -1630,14 +1636,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.81640625" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1648,7 +1654,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1659,7 +1665,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1670,7 +1676,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1681,7 +1687,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1692,7 +1698,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1703,7 +1709,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1714,7 +1720,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1725,7 +1731,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1736,7 +1742,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1747,7 +1753,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1758,7 +1764,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1769,7 +1775,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1780,7 +1786,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1791,7 +1797,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1802,7 +1808,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1813,7 +1819,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1824,7 +1830,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1835,7 +1841,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1846,7 +1852,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1874,20 +1880,20 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="24.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1904,7 +1910,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>99</v>
       </c>
@@ -1918,7 +1924,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1932,7 +1938,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>101</v>
       </c>
@@ -1946,7 +1952,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -1960,7 +1966,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>104</v>
       </c>
@@ -1974,7 +1980,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -1988,7 +1994,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>102</v>
       </c>
@@ -2002,7 +2008,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -2016,7 +2022,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -2030,7 +2036,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>113</v>
       </c>
@@ -2044,7 +2050,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>249</v>
       </c>
@@ -2058,7 +2064,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -2072,7 +2078,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>258</v>
       </c>
@@ -2086,7 +2092,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>117</v>
       </c>
@@ -2100,7 +2106,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>118</v>
       </c>
@@ -2114,7 +2120,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>250</v>
       </c>
@@ -2128,7 +2134,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -2142,7 +2148,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>123</v>
       </c>
@@ -2156,7 +2162,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -2170,7 +2176,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>160</v>
       </c>
@@ -2184,7 +2190,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>162</v>
       </c>
@@ -2198,7 +2204,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>217</v>
       </c>
@@ -2212,7 +2218,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>251</v>
       </c>
@@ -2226,7 +2232,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>166</v>
       </c>
@@ -2240,7 +2246,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>168</v>
       </c>
@@ -2254,7 +2260,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>170</v>
       </c>
@@ -2268,7 +2274,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>172</v>
       </c>
@@ -2282,7 +2288,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>174</v>
       </c>
@@ -2296,7 +2302,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>176</v>
       </c>
@@ -2310,7 +2316,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>177</v>
       </c>
@@ -2324,7 +2330,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>180</v>
       </c>
@@ -2338,7 +2344,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>182</v>
       </c>
@@ -2352,7 +2358,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>184</v>
       </c>
@@ -2366,7 +2372,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>164</v>
       </c>
@@ -2380,7 +2386,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>165</v>
       </c>
@@ -2394,7 +2400,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>186</v>
       </c>
@@ -2408,7 +2414,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>188</v>
       </c>
@@ -2422,7 +2428,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>189</v>
       </c>
@@ -2436,7 +2442,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>197</v>
       </c>
@@ -2450,7 +2456,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>199</v>
       </c>
@@ -2464,7 +2470,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>200</v>
       </c>
@@ -2478,7 +2484,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>191</v>
       </c>
@@ -2492,7 +2498,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>192</v>
       </c>
@@ -2506,7 +2512,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>203</v>
       </c>
@@ -2520,7 +2526,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>206</v>
       </c>
@@ -2534,7 +2540,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>207</v>
       </c>
@@ -2548,7 +2554,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>209</v>
       </c>
@@ -2562,7 +2568,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>211</v>
       </c>
@@ -2576,7 +2582,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>213</v>
       </c>
@@ -2590,7 +2596,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>214</v>
       </c>
@@ -2621,23 +2627,23 @@
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="26.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2663,7 +2669,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -2689,7 +2695,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -2715,7 +2721,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -2741,7 +2747,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2767,7 +2773,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -2793,7 +2799,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -2810,7 +2816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -2836,7 +2842,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -2862,7 +2868,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -2879,7 +2885,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -2896,7 +2902,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2913,7 +2919,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -2930,7 +2936,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -2947,7 +2953,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2964,7 +2970,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -2981,7 +2987,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -2998,7 +3004,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -3015,7 +3021,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -3032,7 +3038,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -3049,7 +3055,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -3066,7 +3072,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -3083,7 +3089,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -3100,7 +3106,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -3117,7 +3123,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -3134,7 +3140,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -3151,7 +3157,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -3168,7 +3174,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -3185,7 +3191,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>246</v>
       </c>
@@ -3199,7 +3205,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>247</v>
       </c>
@@ -3230,20 +3236,20 @@
       <selection activeCell="E8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -3260,7 +3266,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -3274,7 +3280,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>131</v>
       </c>
@@ -3288,7 +3294,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -3302,7 +3308,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>129</v>
       </c>
@@ -3316,7 +3322,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>128</v>
       </c>
@@ -3330,7 +3336,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -3344,7 +3350,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>96</v>
       </c>
@@ -3358,7 +3364,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -3372,7 +3378,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>134</v>
       </c>
@@ -3386,7 +3392,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>133</v>
       </c>
@@ -3400,7 +3406,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>125</v>
       </c>
@@ -3414,7 +3420,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -3428,7 +3434,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>127</v>
       </c>
@@ -3442,7 +3448,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -3456,7 +3462,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>141</v>
       </c>
@@ -3470,7 +3476,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -3484,7 +3490,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -3498,7 +3504,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>138</v>
       </c>
@@ -3512,7 +3518,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>142</v>
       </c>
@@ -3526,7 +3532,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>143</v>
       </c>
@@ -3557,16 +3563,16 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.26953125" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>244</v>
       </c>
@@ -3580,7 +3586,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -3594,7 +3600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -3608,7 +3614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -3622,7 +3628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -3636,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -3650,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -3681,13 +3687,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>269</v>
       </c>
@@ -3695,7 +3701,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>282</v>
       </c>
@@ -3703,7 +3709,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>289</v>
       </c>
@@ -3711,7 +3717,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>280</v>
       </c>
@@ -3719,7 +3725,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>280</v>
       </c>
@@ -3727,7 +3733,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>312</v>
       </c>
@@ -3735,7 +3741,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>272</v>
       </c>
@@ -3743,7 +3749,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>287</v>
       </c>
@@ -3751,7 +3757,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>277</v>
       </c>
@@ -3759,7 +3765,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>279</v>
       </c>
@@ -3767,7 +3773,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>291</v>
       </c>
@@ -3775,7 +3781,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>284</v>
       </c>
@@ -3783,7 +3789,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>271</v>
       </c>
@@ -3791,7 +3797,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>274</v>
       </c>
@@ -3799,7 +3805,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>285</v>
       </c>
@@ -3807,7 +3813,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>309</v>
       </c>
@@ -3825,19 +3831,21 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2F7ED2-3887-47C4-B9C3-26B3456EF3BF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>315</v>
       </c>
@@ -3850,8 +3858,11 @@
       <c r="D1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>316</v>
       </c>
@@ -3860,6 +3871,9 @@
       </c>
       <c r="D2" t="s">
         <v>313</v>
+      </c>
+      <c r="E2" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove event_name_edc from metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D0675C-A27D-49A3-B464-7A47CEC1DC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0550EC7-05B4-48B2-BC9C-E9C70A8A6F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="298">
   <si>
     <t>continuous</t>
   </si>
@@ -968,12 +968,6 @@
   </si>
   <si>
     <t>^UN</t>
-  </si>
-  <si>
-    <t>EventName</t>
-  </si>
-  <si>
-    <t>event_name_edc</t>
   </si>
 </sst>
 </file>
@@ -1054,8 +1048,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}" name="Table7" displayName="Table7" ref="A1:B12" totalsRowShown="0">
-  <autoFilter ref="A1:B12" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}" name="Table7" displayName="Table7" ref="A1:B11" totalsRowShown="0">
+  <autoFilter ref="A1:B11" xr:uid="{3DA32AC3-4A18-4922-894E-765CD043E044}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{197420D8-A12C-4324-87A4-2BEAC3F2FAF6}" name="name_raw"/>
     <tableColumn id="2" xr3:uid="{9CEB246F-9418-43C1-93E4-E01091B6A441}" name="name_new"/>
@@ -1452,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A2BBF1-D698-4542-9229-382D48A2C041}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,14 +1544,6 @@
       </c>
       <c r="B11" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>298</v>
-      </c>
-      <c r="B12" t="s">
-        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -1572,7 +1558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD7656C-2CDB-4668-9193-1FF1E214725D}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update docs and improve metadata$events column names
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0550EC7-05B4-48B2-BC9C-E9C70A8A6F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A7620C-32CD-4537-B780-487F008F2C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -922,21 +922,9 @@
     <t>apply_edc_specific_changes</t>
   </si>
   <si>
-    <t>visit_name</t>
-  </si>
-  <si>
-    <t>visit_suffix</t>
-  </si>
-  <si>
     <t>event_id_pattern</t>
   </si>
   <si>
-    <t>is_visit_day</t>
-  </si>
-  <si>
-    <t>max_n_events</t>
-  </si>
-  <si>
     <t>^SCR</t>
   </si>
   <si>
@@ -968,6 +956,18 @@
   </si>
   <si>
     <t>^UN</t>
+  </si>
+  <si>
+    <t>event_prefix</t>
+  </si>
+  <si>
+    <t>event_suffix</t>
+  </si>
+  <si>
+    <t>is_scheduled_visit</t>
+  </si>
+  <si>
+    <t>expected_events</t>
   </si>
 </sst>
 </file>
@@ -1062,11 +1062,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38272256-CB6A-401F-A9BB-4ADF1E6D0056}" name="Table9" displayName="Table9" ref="A1:E7" totalsRowShown="0">
   <autoFilter ref="A1:E7" xr:uid="{5E91F354-8F5C-479A-B965-FD3A5DC02CD5}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2AD6F31B-93AD-4ED7-8C3B-E09A3EEBCD38}" name="visit_name"/>
-    <tableColumn id="2" xr3:uid="{27889339-640B-4E62-B6DD-4652B73E1551}" name="visit_suffix"/>
+    <tableColumn id="1" xr3:uid="{2AD6F31B-93AD-4ED7-8C3B-E09A3EEBCD38}" name="event_prefix"/>
+    <tableColumn id="2" xr3:uid="{27889339-640B-4E62-B6DD-4652B73E1551}" name="event_suffix"/>
     <tableColumn id="3" xr3:uid="{9C22BAFC-4258-45F1-BFA1-1BF97E03A54C}" name="event_id_pattern"/>
-    <tableColumn id="4" xr3:uid="{FE5140BE-58FF-4D6F-A810-3EFF5B533384}" name="is_visit_day"/>
-    <tableColumn id="5" xr3:uid="{3E9E291E-A833-400C-9F16-AD7B8A1854B0}" name="max_n_events"/>
+    <tableColumn id="4" xr3:uid="{FE5140BE-58FF-4D6F-A810-3EFF5B533384}" name="is_scheduled_visit"/>
+    <tableColumn id="5" xr3:uid="{3E9E291E-A833-400C-9F16-AD7B8A1854B0}" name="expected_events"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1448,9 +1448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A2BBF1-D698-4542-9229-382D48A2C041}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1558,34 +1556,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD7656C-2CDB-4668-9193-1FF1E214725D}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" t="s">
         <v>282</v>
       </c>
-      <c r="B1" t="s">
-        <v>283</v>
-      </c>
-      <c r="C1" t="s">
-        <v>284</v>
-      </c>
       <c r="D1" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="E1" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1593,7 +1591,7 @@
         <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1604,10 +1602,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1618,13 +1616,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C4" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1632,13 +1630,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B5" t="s">
         <v>288</v>
       </c>
-      <c r="B5" t="s">
-        <v>292</v>
-      </c>
       <c r="C5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -1646,10 +1644,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C6" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -1660,10 +1658,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
@@ -3037,9 +3035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D649F3-3138-4439-A355-CAB4EEAE2B78}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="A8:E8"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3365,7 +3361,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ensure event_labels in compact timeline are flexible again
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A7620C-32CD-4537-B780-487F008F2C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910D5765-6FF7-4CD0-97ED-345BBE1B259B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="300">
   <si>
     <t>continuous</t>
   </si>
@@ -968,6 +968,12 @@
   </si>
   <si>
     <t>expected_events</t>
+  </si>
+  <si>
+    <t>SCR</t>
+  </si>
+  <si>
+    <t>C1D1</t>
   </si>
 </sst>
 </file>
@@ -1059,11 +1065,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38272256-CB6A-401F-A9BB-4ADF1E6D0056}" name="Table9" displayName="Table9" ref="A1:E7" totalsRowShown="0">
-  <autoFilter ref="A1:E7" xr:uid="{5E91F354-8F5C-479A-B965-FD3A5DC02CD5}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38272256-CB6A-401F-A9BB-4ADF1E6D0056}" name="Table9" displayName="Table9" ref="A1:F7" totalsRowShown="0">
+  <autoFilter ref="A1:F7" xr:uid="{5E91F354-8F5C-479A-B965-FD3A5DC02CD5}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2AD6F31B-93AD-4ED7-8C3B-E09A3EEBCD38}" name="event_prefix"/>
     <tableColumn id="2" xr3:uid="{27889339-640B-4E62-B6DD-4652B73E1551}" name="event_suffix"/>
+    <tableColumn id="6" xr3:uid="{CC3A9CD9-5C07-4028-BB20-18D01844693A}" name="event_id"/>
     <tableColumn id="3" xr3:uid="{9C22BAFC-4258-45F1-BFA1-1BF97E03A54C}" name="event_id_pattern"/>
     <tableColumn id="4" xr3:uid="{FE5140BE-58FF-4D6F-A810-3EFF5B533384}" name="is_scheduled_visit"/>
     <tableColumn id="5" xr3:uid="{3E9E291E-A833-400C-9F16-AD7B8A1854B0}" name="expected_events"/>
@@ -1554,22 +1561,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD7656C-2CDB-4668-9193-1FF1E214725D}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>294</v>
       </c>
@@ -1577,93 +1585,102 @@
         <v>295</v>
       </c>
       <c r="C1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1" t="s">
         <v>282</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>296</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>201</v>
       </c>
       <c r="C2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D2" t="s">
         <v>283</v>
       </c>
-      <c r="D2" t="b">
+      <c r="E2" t="b">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>284</v>
       </c>
       <c r="C3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" t="s">
         <v>285</v>
       </c>
-      <c r="D3" t="b">
+      <c r="E3" t="b">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>284</v>
       </c>
       <c r="B4" t="s">
         <v>286</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>287</v>
       </c>
-      <c r="D4" t="b">
+      <c r="E4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>284</v>
       </c>
       <c r="B5" t="s">
         <v>288</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>289</v>
       </c>
-      <c r="D5" t="b">
+      <c r="E5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>290</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>291</v>
       </c>
-      <c r="D6" t="b">
+      <c r="E6" t="b">
         <v>0</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>292</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>293</v>
       </c>
-      <c r="D7" t="b">
+      <c r="E7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3634,7 +3651,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2F7ED2-3887-47C4-B9C3-26B3456EF3BF}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Simplify code and fix it for one study
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8612A2C-DD48-4ACE-9228-3F9F20198C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A16156-4083-4732-9BB4-B9FEDD275D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="298">
   <si>
     <t>continuous</t>
   </si>
@@ -958,26 +958,23 @@
     <t>^UN</t>
   </si>
   <si>
-    <t>event_prefix</t>
-  </si>
-  <si>
-    <t>event_suffix</t>
-  </si>
-  <si>
-    <t>is_scheduled_visit</t>
-  </si>
-  <si>
-    <t>min_expected_visits</t>
-  </si>
-  <si>
     <t>add_event_number</t>
+  </si>
+  <si>
+    <t>event_name_prefix</t>
+  </si>
+  <si>
+    <t>event_name_suffix</t>
+  </si>
+  <si>
+    <t>expected_visits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -991,13 +988,37 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1012,16 +1033,76 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1062,16 +1143,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38272256-CB6A-401F-A9BB-4ADF1E6D0056}" name="Table9" displayName="Table9" ref="A1:G7" totalsRowShown="0">
-  <autoFilter ref="A1:G7" xr:uid="{5E91F354-8F5C-479A-B965-FD3A5DC02CD5}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2AD6F31B-93AD-4ED7-8C3B-E09A3EEBCD38}" name="event_prefix"/>
-    <tableColumn id="2" xr3:uid="{27889339-640B-4E62-B6DD-4652B73E1551}" name="event_suffix"/>
-    <tableColumn id="6" xr3:uid="{CC3A9CD9-5C07-4028-BB20-18D01844693A}" name="event_id"/>
-    <tableColumn id="3" xr3:uid="{9C22BAFC-4258-45F1-BFA1-1BF97E03A54C}" name="event_id_pattern"/>
-    <tableColumn id="4" xr3:uid="{FE5140BE-58FF-4D6F-A810-3EFF5B533384}" name="is_scheduled_visit"/>
-    <tableColumn id="5" xr3:uid="{3E9E291E-A833-400C-9F16-AD7B8A1854B0}" name="min_expected_visits"/>
-    <tableColumn id="7" xr3:uid="{2D304B6A-5D88-45CC-A4B6-8F3BFD1F1C5D}" name="add_event_number"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38272256-CB6A-401F-A9BB-4ADF1E6D0056}" name="Table9" displayName="Table9" ref="A1:F7" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="A1:F7" xr:uid="{5E91F354-8F5C-479A-B965-FD3A5DC02CD5}"/>
+  <tableColumns count="6">
+    <tableColumn id="6" xr3:uid="{CC3A9CD9-5C07-4028-BB20-18D01844693A}" name="event_id" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{9C22BAFC-4258-45F1-BFA1-1BF97E03A54C}" name="event_id_pattern" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{3E9E291E-A833-400C-9F16-AD7B8A1854B0}" name="expected_visits" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2AD6F31B-93AD-4ED7-8C3B-E09A3EEBCD38}" name="event_name_prefix" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{27889339-640B-4E62-B6DD-4652B73E1551}" name="event_name_suffix" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{2D304B6A-5D88-45CC-A4B6-8F3BFD1F1C5D}" name="add_event_number" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1082,7 +1162,7 @@
   <autoFilter ref="A1:E51" xr:uid="{3DC8495A-80F1-47D0-B099-A4444169C84F}"/>
   <tableColumns count="5">
     <tableColumn id="12" xr3:uid="{32D2D5DB-90F1-452A-A407-9958F05DFC29}" name="var"/>
-    <tableColumn id="11" xr3:uid="{0CFD0054-C78B-4015-9FD5-17E69E3DF3D4}" name="suffix" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{0CFD0054-C78B-4015-9FD5-17E69E3DF3D4}" name="suffix" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{DDF6B9DA-22E8-4772-BC2A-2E79D78BA24F}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{78F87B1B-3FB5-4BDA-8075-9F2908D15BE4}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{D15D9292-219E-4D48-9449-CA4B7E84D719}" name="item_group"/>
@@ -1099,13 +1179,13 @@
   </sortState>
   <tableColumns count="8">
     <tableColumn id="12" xr3:uid="{3F460AD3-FCC0-44D5-BBE7-96068C605604}" name="var"/>
-    <tableColumn id="11" xr3:uid="{CBDC5ABF-E118-45AB-B067-09A03A7B4DFE}" name="suffix" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{CBDC5ABF-E118-45AB-B067-09A03A7B4DFE}" name="suffix" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{CFD88543-6276-40D6-9487-D6A7385190F4}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{E0E61225-3F35-4968-A99C-26C9994CEE9F}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{9E97B4D1-3E86-442C-9084-2E44749A5442}" name="item_group"/>
     <tableColumn id="4" xr3:uid="{17ACC2A8-A45A-49FD-AC66-881A4CCD7E07}" name="unit"/>
-    <tableColumn id="5" xr3:uid="{C1210F5F-D092-4DE2-8C8C-CB16E4C8274D}" name="lower_limit" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{A093D2B4-AC02-4F13-95A0-F9DE47382C30}" name="upper_limit" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{C1210F5F-D092-4DE2-8C8C-CB16E4C8274D}" name="lower_limit" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{A093D2B4-AC02-4F13-95A0-F9DE47382C30}" name="upper_limit" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1118,7 +1198,7 @@
   </sortState>
   <tableColumns count="5">
     <tableColumn id="12" xr3:uid="{5604E1C1-7286-42A9-9446-BD07C4022CD9}" name="var"/>
-    <tableColumn id="11" xr3:uid="{BEFC1292-D34C-4190-BD53-E5DB8DEA8068}" name="suffix" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{BEFC1292-D34C-4190-BD53-E5DB8DEA8068}" name="suffix" dataDxfId="7"/>
     <tableColumn id="10" xr3:uid="{EE82524D-5440-46D2-ABCD-5FFB7844C279}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{29DD0374-4740-492E-9A7C-90F52163213A}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{F6C07853-FBDF-4C62-8817-4C93F651B74A}" name="item_group"/>
@@ -1559,152 +1639,140 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD7656C-2CDB-4668-9193-1FF1E214725D}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E1" t="s">
-        <v>296</v>
-      </c>
-      <c r="F1" t="s">
-        <v>297</v>
-      </c>
-      <c r="G1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E2" t="b">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C3" s="4">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C4" s="4">
         <v>1</v>
       </c>
-      <c r="G2" t="b">
+      <c r="D4" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="F4" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F5" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D3" t="s">
-        <v>285</v>
-      </c>
-      <c r="E3" t="b">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>17</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>284</v>
-      </c>
-      <c r="B4" t="s">
-        <v>286</v>
-      </c>
-      <c r="D4" t="s">
-        <v>287</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>284</v>
-      </c>
-      <c r="B5" t="s">
-        <v>288</v>
-      </c>
-      <c r="D5" t="s">
-        <v>289</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>290</v>
-      </c>
-      <c r="D6" t="s">
-        <v>291</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>292</v>
-      </c>
-      <c r="D7" t="s">
-        <v>293</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1717,13 +1785,13 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Create some fixes to work with clinsight internal data
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A16156-4083-4732-9BB4-B9FEDD275D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AE16B3-B436-47C3-9EB4-4EE99808A51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
-    <sheet name="events" sheetId="20" r:id="rId2"/>
+    <sheet name="events" sheetId="21" r:id="rId2"/>
     <sheet name="common_forms" sheetId="13" r:id="rId3"/>
     <sheet name="study_forms" sheetId="14" r:id="rId4"/>
     <sheet name="general" sheetId="15" r:id="rId5"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="297">
   <si>
     <t>continuous</t>
   </si>
@@ -925,56 +925,53 @@
     <t>event_id_pattern</t>
   </si>
   <si>
-    <t>^SCR</t>
-  </si>
-  <si>
     <t>Visit</t>
   </si>
   <si>
     <t>^VIS</t>
   </si>
   <si>
-    <t>FU</t>
-  </si>
-  <si>
     <t>^FU</t>
   </si>
   <si>
     <t>EoT</t>
   </si>
   <si>
-    <t>^EOT$</t>
-  </si>
-  <si>
     <t>Exit</t>
   </si>
   <si>
-    <t>^EXIT</t>
-  </si>
-  <si>
     <t>Unscheduled visit</t>
   </si>
   <si>
     <t>^UN</t>
   </si>
   <si>
-    <t>add_event_number</t>
-  </si>
-  <si>
-    <t>event_name_prefix</t>
-  </si>
-  <si>
-    <t>event_name_suffix</t>
-  </si>
-  <si>
-    <t>expected_visits</t>
+    <t>is_expected_visit</t>
+  </si>
+  <si>
+    <t>event_label_custom</t>
+  </si>
+  <si>
+    <t>event_name_custom</t>
+  </si>
+  <si>
+    <t>add_sequence_to_name</t>
+  </si>
+  <si>
+    <t>SCR</t>
+  </si>
+  <si>
+    <t>EOT</t>
+  </si>
+  <si>
+    <t>EXIT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -988,25 +985,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1016,7 +1001,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1033,75 +1018,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="6">
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1143,15 +1076,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38272256-CB6A-401F-A9BB-4ADF1E6D0056}" name="Table9" displayName="Table9" ref="A1:F7" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AF0B2251-C975-4933-824C-576F9F542B56}" name="Table913" displayName="Table913" ref="A1:F7" totalsRowShown="0">
   <autoFilter ref="A1:F7" xr:uid="{5E91F354-8F5C-479A-B965-FD3A5DC02CD5}"/>
   <tableColumns count="6">
-    <tableColumn id="6" xr3:uid="{CC3A9CD9-5C07-4028-BB20-18D01844693A}" name="event_id" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{9C22BAFC-4258-45F1-BFA1-1BF97E03A54C}" name="event_id_pattern" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{3E9E291E-A833-400C-9F16-AD7B8A1854B0}" name="expected_visits" dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{2AD6F31B-93AD-4ED7-8C3B-E09A3EEBCD38}" name="event_name_prefix" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{27889339-640B-4E62-B6DD-4652B73E1551}" name="event_name_suffix" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{2D304B6A-5D88-45CC-A4B6-8F3BFD1F1C5D}" name="add_event_number" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{23B237DE-B09E-44C0-BAB0-6FAD4E8B82E1}" name="event_id"/>
+    <tableColumn id="3" xr3:uid="{E4972731-D21F-4F99-8ED7-12BC30CAAE58}" name="event_id_pattern"/>
+    <tableColumn id="5" xr3:uid="{9904954A-4F18-4879-A696-2928DD7B4B4D}" name="is_expected_visit" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{EB5F1517-6D17-406D-B40D-7A226BCB0152}" name="event_label_custom"/>
+    <tableColumn id="1" xr3:uid="{D00CCD3C-0B83-4F62-819D-2252C93BACA1}" name="event_name_custom"/>
+    <tableColumn id="4" xr3:uid="{BB03C888-0BDD-43BA-9A30-18761267B7B6}" name="add_sequence_to_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1162,7 +1095,7 @@
   <autoFilter ref="A1:E51" xr:uid="{3DC8495A-80F1-47D0-B099-A4444169C84F}"/>
   <tableColumns count="5">
     <tableColumn id="12" xr3:uid="{32D2D5DB-90F1-452A-A407-9958F05DFC29}" name="var"/>
-    <tableColumn id="11" xr3:uid="{0CFD0054-C78B-4015-9FD5-17E69E3DF3D4}" name="suffix" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{0CFD0054-C78B-4015-9FD5-17E69E3DF3D4}" name="suffix" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{DDF6B9DA-22E8-4772-BC2A-2E79D78BA24F}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{78F87B1B-3FB5-4BDA-8075-9F2908D15BE4}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{D15D9292-219E-4D48-9449-CA4B7E84D719}" name="item_group"/>
@@ -1179,13 +1112,13 @@
   </sortState>
   <tableColumns count="8">
     <tableColumn id="12" xr3:uid="{3F460AD3-FCC0-44D5-BBE7-96068C605604}" name="var"/>
-    <tableColumn id="11" xr3:uid="{CBDC5ABF-E118-45AB-B067-09A03A7B4DFE}" name="suffix" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{CBDC5ABF-E118-45AB-B067-09A03A7B4DFE}" name="suffix" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{CFD88543-6276-40D6-9487-D6A7385190F4}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{E0E61225-3F35-4968-A99C-26C9994CEE9F}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{9E97B4D1-3E86-442C-9084-2E44749A5442}" name="item_group"/>
     <tableColumn id="4" xr3:uid="{17ACC2A8-A45A-49FD-AC66-881A4CCD7E07}" name="unit"/>
-    <tableColumn id="5" xr3:uid="{C1210F5F-D092-4DE2-8C8C-CB16E4C8274D}" name="lower_limit" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{A093D2B4-AC02-4F13-95A0-F9DE47382C30}" name="upper_limit" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{C1210F5F-D092-4DE2-8C8C-CB16E4C8274D}" name="lower_limit" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{A093D2B4-AC02-4F13-95A0-F9DE47382C30}" name="upper_limit" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1198,7 +1131,7 @@
   </sortState>
   <tableColumns count="5">
     <tableColumn id="12" xr3:uid="{5604E1C1-7286-42A9-9446-BD07C4022CD9}" name="var"/>
-    <tableColumn id="11" xr3:uid="{BEFC1292-D34C-4190-BD53-E5DB8DEA8068}" name="suffix" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{BEFC1292-D34C-4190-BD53-E5DB8DEA8068}" name="suffix" dataDxfId="1"/>
     <tableColumn id="10" xr3:uid="{EE82524D-5440-46D2-ABCD-5FFB7844C279}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{29DD0374-4740-492E-9A7C-90F52163213A}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{F6C07853-FBDF-4C62-8817-4C93F651B74A}" name="item_group"/>
@@ -1638,141 +1571,132 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD7656C-2CDB-4668-9193-1FF1E214725D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3EAE6FA-BABD-4471-8238-77F95F9C10BF}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>283</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>295</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="C4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" t="s">
+        <v>286</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>296</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="C6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>287</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>288</v>
+      </c>
+      <c r="F7" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="C3" s="4">
-        <v>17</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="F4" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="F5" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="b">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Update metadata after merge conflict
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AE16B3-B436-47C3-9EB4-4EE99808A51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680AFC4B-D909-4250-9A35-1721D36E6649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="3435" yWindow="3240" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
-    <sheet name="events" sheetId="21" r:id="rId2"/>
+    <sheet name="events" sheetId="19" r:id="rId2"/>
     <sheet name="common_forms" sheetId="13" r:id="rId3"/>
     <sheet name="study_forms" sheetId="14" r:id="rId4"/>
     <sheet name="general" sheetId="15" r:id="rId5"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="299">
   <si>
     <t>continuous</t>
   </si>
@@ -922,49 +922,55 @@
     <t>apply_edc_specific_changes</t>
   </si>
   <si>
+    <t>treatment_label</t>
+  </si>
+  <si>
+    <t>\U1F48A T\U2093</t>
+  </si>
+  <si>
     <t>event_id_pattern</t>
   </si>
   <si>
+    <t>is_expected_visit</t>
+  </si>
+  <si>
+    <t>event_label_custom</t>
+  </si>
+  <si>
+    <t>event_name_custom</t>
+  </si>
+  <si>
+    <t>add_sequence_to_name</t>
+  </si>
+  <si>
+    <t>SCR</t>
+  </si>
+  <si>
+    <t>^VIS</t>
+  </si>
+  <si>
     <t>Visit</t>
   </si>
   <si>
-    <t>^VIS</t>
+    <t>EOT</t>
+  </si>
+  <si>
+    <t>EoT</t>
   </si>
   <si>
     <t>^FU</t>
   </si>
   <si>
-    <t>EoT</t>
+    <t>EXIT</t>
   </si>
   <si>
     <t>Exit</t>
   </si>
   <si>
+    <t>^UN</t>
+  </si>
+  <si>
     <t>Unscheduled visit</t>
-  </si>
-  <si>
-    <t>^UN</t>
-  </si>
-  <si>
-    <t>is_expected_visit</t>
-  </si>
-  <si>
-    <t>event_label_custom</t>
-  </si>
-  <si>
-    <t>event_name_custom</t>
-  </si>
-  <si>
-    <t>add_sequence_to_name</t>
-  </si>
-  <si>
-    <t>SCR</t>
-  </si>
-  <si>
-    <t>EOT</t>
-  </si>
-  <si>
-    <t>EXIT</t>
   </si>
 </sst>
 </file>
@@ -995,13 +1001,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1034,9 +1040,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1050,6 +1053,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1076,15 +1082,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{AF0B2251-C975-4933-824C-576F9F542B56}" name="Table913" displayName="Table913" ref="A1:F7" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FAB0EA66-5868-4938-9FA9-F93E72C101B3}" name="Table913" displayName="Table913" ref="A1:F7" totalsRowShown="0">
   <autoFilter ref="A1:F7" xr:uid="{5E91F354-8F5C-479A-B965-FD3A5DC02CD5}"/>
   <tableColumns count="6">
-    <tableColumn id="6" xr3:uid="{23B237DE-B09E-44C0-BAB0-6FAD4E8B82E1}" name="event_id"/>
-    <tableColumn id="3" xr3:uid="{E4972731-D21F-4F99-8ED7-12BC30CAAE58}" name="event_id_pattern"/>
-    <tableColumn id="5" xr3:uid="{9904954A-4F18-4879-A696-2928DD7B4B4D}" name="is_expected_visit" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{EB5F1517-6D17-406D-B40D-7A226BCB0152}" name="event_label_custom"/>
-    <tableColumn id="1" xr3:uid="{D00CCD3C-0B83-4F62-819D-2252C93BACA1}" name="event_name_custom"/>
-    <tableColumn id="4" xr3:uid="{BB03C888-0BDD-43BA-9A30-18761267B7B6}" name="add_sequence_to_name"/>
+    <tableColumn id="6" xr3:uid="{E993CBC8-A1B1-4E4C-8906-7171AD5EB8DA}" name="event_id"/>
+    <tableColumn id="3" xr3:uid="{2C30F1DE-E33C-48DF-B5EA-F221EFC19502}" name="event_id_pattern"/>
+    <tableColumn id="5" xr3:uid="{B8744317-3956-4F39-A2A1-F571FB40341F}" name="is_expected_visit" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{BC267C30-A507-48B0-8B2A-ABC6EB4A6D66}" name="event_label_custom"/>
+    <tableColumn id="1" xr3:uid="{76BD4AA6-095B-46B4-AD1F-74CB4B63B7A1}" name="event_name_custom"/>
+    <tableColumn id="4" xr3:uid="{BC23E39F-CE6F-4D20-AF70-E0E9D2B9A5E8}" name="add_sequence_to_name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1095,7 +1101,7 @@
   <autoFilter ref="A1:E51" xr:uid="{3DC8495A-80F1-47D0-B099-A4444169C84F}"/>
   <tableColumns count="5">
     <tableColumn id="12" xr3:uid="{32D2D5DB-90F1-452A-A407-9958F05DFC29}" name="var"/>
-    <tableColumn id="11" xr3:uid="{0CFD0054-C78B-4015-9FD5-17E69E3DF3D4}" name="suffix" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{0CFD0054-C78B-4015-9FD5-17E69E3DF3D4}" name="suffix" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{DDF6B9DA-22E8-4772-BC2A-2E79D78BA24F}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{78F87B1B-3FB5-4BDA-8075-9F2908D15BE4}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{D15D9292-219E-4D48-9449-CA4B7E84D719}" name="item_group"/>
@@ -1112,13 +1118,13 @@
   </sortState>
   <tableColumns count="8">
     <tableColumn id="12" xr3:uid="{3F460AD3-FCC0-44D5-BBE7-96068C605604}" name="var"/>
-    <tableColumn id="11" xr3:uid="{CBDC5ABF-E118-45AB-B067-09A03A7B4DFE}" name="suffix" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{CBDC5ABF-E118-45AB-B067-09A03A7B4DFE}" name="suffix" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{CFD88543-6276-40D6-9487-D6A7385190F4}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{E0E61225-3F35-4968-A99C-26C9994CEE9F}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{9E97B4D1-3E86-442C-9084-2E44749A5442}" name="item_group"/>
     <tableColumn id="4" xr3:uid="{17ACC2A8-A45A-49FD-AC66-881A4CCD7E07}" name="unit"/>
-    <tableColumn id="5" xr3:uid="{C1210F5F-D092-4DE2-8C8C-CB16E4C8274D}" name="lower_limit" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{A093D2B4-AC02-4F13-95A0-F9DE47382C30}" name="upper_limit" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{C1210F5F-D092-4DE2-8C8C-CB16E4C8274D}" name="lower_limit" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{A093D2B4-AC02-4F13-95A0-F9DE47382C30}" name="upper_limit" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1131,7 +1137,7 @@
   </sortState>
   <tableColumns count="5">
     <tableColumn id="12" xr3:uid="{5604E1C1-7286-42A9-9446-BD07C4022CD9}" name="var"/>
-    <tableColumn id="11" xr3:uid="{BEFC1292-D34C-4190-BD53-E5DB8DEA8068}" name="suffix" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{BEFC1292-D34C-4190-BD53-E5DB8DEA8068}" name="suffix" dataDxfId="0"/>
     <tableColumn id="10" xr3:uid="{EE82524D-5440-46D2-ABCD-5FFB7844C279}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{29DD0374-4740-492E-9A7C-90F52163213A}" name="item_type"/>
     <tableColumn id="8" xr3:uid="{F6C07853-FBDF-4C62-8817-4C93F651B74A}" name="item_group"/>
@@ -1471,7 +1477,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1571,12 +1577,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3EAE6FA-BABD-4471-8238-77F95F9C10BF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47507AE3-65CF-4352-8C5A-A70367C9C41D}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1590,28 +1594,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>293</v>
+      <c r="B1" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C2" s="4" t="b">
         <v>1</v>
@@ -1625,13 +1629,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -1639,16 +1643,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="E4" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1656,13 +1660,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -1670,13 +1674,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
         <v>296</v>
-      </c>
-      <c r="C6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>287</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1684,13 +1688,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -1709,13 +1713,13 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -3064,7 +3068,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D649F3-3138-4439-A355-CAB4EEAE2B78}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="A8:E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3390,7 +3396,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3661,21 +3667,21 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2F7ED2-3887-47C4-B9C3-26B3456EF3BF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>277</v>
       </c>
@@ -3688,8 +3694,11 @@
       <c r="D1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>278</v>
       </c>
@@ -3698,6 +3707,9 @@
       </c>
       <c r="D2" t="s">
         <v>275</v>
+      </c>
+      <c r="E2" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update metadata to reflect the new state
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFA5280-21A6-41FA-A04B-F57EC55E69B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B8246A-141E-466F-B194-245DBE4B06EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
   <sheets>
     <sheet name="column_names" sheetId="17" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="301">
   <si>
     <t>continuous</t>
   </si>
@@ -940,9 +940,6 @@
     <t>SCR</t>
   </si>
   <si>
-    <t>^VIS</t>
-  </si>
-  <si>
     <t>Visit</t>
   </si>
   <si>
@@ -971,6 +968,15 @@
   </si>
   <si>
     <t>is_baseline_event</t>
+  </si>
+  <si>
+    <t>FU</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>^VIS[[:digit:]]+$</t>
   </si>
 </sst>
 </file>
@@ -1472,7 +1478,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A2BBF1-D698-4542-9229-382D48A2C041}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1580,9 +1588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47507AE3-65CF-4352-8C5A-A70367C9C41D}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1603,7 +1609,7 @@
         <v>284</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>285</v>
@@ -1612,7 +1618,7 @@
         <v>286</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1631,13 +1637,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>1</v>
       </c>
+      <c r="D3" t="s">
+        <v>299</v>
+      </c>
       <c r="E3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1645,16 +1654,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
@@ -1662,13 +1671,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>1</v>
       </c>
+      <c r="D5" t="s">
+        <v>298</v>
+      </c>
       <c r="E5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1676,13 +1688,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>292</v>
+      </c>
+      <c r="C6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
         <v>293</v>
-      </c>
-      <c r="C6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>294</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1690,13 +1702,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
         <v>295</v>
-      </c>
-      <c r="C7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>296</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Update metadata events to primarily use event_id instead of event_id_pattern
</commit_message>
<xml_diff>
--- a/data-raw/metadata.xlsx
+++ b/data-raw/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lsamson\Projects\99 - Statistial and data projects\IMpress\clinsight\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B8246A-141E-466F-B194-245DBE4B06EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F27630-12B8-4921-B4AE-686264D9EA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3E8FFA66-BACE-4C4A-A255-562C367A8A13}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="314">
   <si>
     <t>continuous</t>
   </si>
@@ -940,18 +940,12 @@
     <t>SCR</t>
   </si>
   <si>
-    <t>Visit</t>
-  </si>
-  <si>
     <t>EOT</t>
   </si>
   <si>
     <t>EoT</t>
   </si>
   <si>
-    <t>^FU</t>
-  </si>
-  <si>
     <t>EXIT</t>
   </si>
   <si>
@@ -970,20 +964,65 @@
     <t>is_baseline_event</t>
   </si>
   <si>
-    <t>FU</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>^VIS[[:digit:]]+$</t>
+    <t>VIS1</t>
+  </si>
+  <si>
+    <t>VIS2</t>
+  </si>
+  <si>
+    <t>VIS3</t>
+  </si>
+  <si>
+    <t>VIS4</t>
+  </si>
+  <si>
+    <t>VIS5</t>
+  </si>
+  <si>
+    <t>VIS6</t>
+  </si>
+  <si>
+    <t>Visit 1</t>
+  </si>
+  <si>
+    <t>Visit 2</t>
+  </si>
+  <si>
+    <t>Visit 3</t>
+  </si>
+  <si>
+    <t>Visit 4</t>
+  </si>
+  <si>
+    <t>Visit 5</t>
+  </si>
+  <si>
+    <t>Visit 6</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>V6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -996,6 +1035,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1088,8 +1133,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FAB0EA66-5868-4938-9FA9-F93E72C101B3}" name="Table913" displayName="Table913" ref="A1:F7" totalsRowShown="0">
-  <autoFilter ref="A1:F7" xr:uid="{5E91F354-8F5C-479A-B965-FD3A5DC02CD5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{FAB0EA66-5868-4938-9FA9-F93E72C101B3}" name="Table913" displayName="Table913" ref="A1:F11" totalsRowShown="0">
+  <autoFilter ref="A1:F11" xr:uid="{5E91F354-8F5C-479A-B965-FD3A5DC02CD5}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{E993CBC8-A1B1-4E4C-8906-7171AD5EB8DA}" name="event_id"/>
     <tableColumn id="3" xr3:uid="{2C30F1DE-E33C-48DF-B5EA-F221EFC19502}" name="event_id_pattern"/>
@@ -1586,14 +1631,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47507AE3-65CF-4352-8C5A-A70367C9C41D}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.453125" bestFit="1" customWidth="1"/>
@@ -1609,7 +1657,7 @@
         <v>284</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>285</v>
@@ -1618,7 +1666,7 @@
         <v>286</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -1636,17 +1684,17 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>300</v>
+      <c r="A3" t="s">
+        <v>296</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="E3" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -1654,33 +1702,33 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
       <c r="E4" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>291</v>
+      <c r="A5" t="s">
+        <v>298</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="E5" t="s">
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1688,33 +1736,102 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>311</v>
+      </c>
+      <c r="E6" t="s">
+        <v>305</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>300</v>
+      </c>
+      <c r="C7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>312</v>
+      </c>
+      <c r="E7" t="s">
+        <v>306</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>301</v>
+      </c>
+      <c r="C8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>313</v>
+      </c>
+      <c r="E8" t="s">
+        <v>307</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E9" t="s">
+        <v>289</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
         <v>292</v>
       </c>
-      <c r="C6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
         <v>293</v>
       </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>294</v>
-      </c>
-      <c r="C7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>295</v>
-      </c>
-      <c r="F7" t="b">
+      <c r="F11" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>